<commit_message>
Fixing Graphs and adding new Forcast Juniper Book Alone
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_MAR_2025.xlsx
+++ b/Monthly_Cost_For_MAR_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.000733608</v>
+        <v>0.0007356137</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.09807092539999999</v>
+        <v>0.1648431505</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>11.458448422</v>
+        <v>17.1435510421</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.0364</v>
+        <v>0.0546</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1456</v>
+        <v>1126.61042676</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>221.0665042311</v>
+        <v>341.3149955157</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>148.0934</v>
+        <v>221.67964</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2.1294</v>
+        <v>2.4479</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.8802115329</v>
+        <v>1.2590381087</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>183.1722365605</v>
+        <v>267.380329249</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>22.795568499</v>
+        <v>32.7427256622</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>36.5438170272</v>
+        <v>52.4658973758</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2.002</v>
+        <v>2.8756</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1.22096e-05</v>
+        <v>1.78448e-05</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.201814514</v>
+        <v>0.2898790292</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>2.5027588691</v>
+        <v>3.5948707742</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.1844730888</v>
+        <v>0.2381931552</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>13.4524668419</v>
+        <v>19.5298095382</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.1321539498</v>
+        <v>0.1920675582</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.06611663819999999</v>
+        <v>0.0955015074</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.06737797650000001</v>
+        <v>0.0967846857</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>5.5276539087</v>
+        <v>7.9670947749</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>4.2906248091</v>
+        <v>6.2882044014</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.0660483882</v>
+        <v>0.0954032274</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.1320967764</v>
+        <v>0.1908064548</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.1323179064</v>
+        <v>0.1911149448</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>104.8533511499</v>
+        <v>171.1901145307</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1477,11 +1477,11 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1.3252034417</v>
+        <v>2.00276e-05</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Development</t>
         </is>
       </c>
     </row>
@@ -1512,11 +1512,11 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0.2328984407</v>
+        <v>1.9678661285</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1547,11 +1547,11 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.1577170139</v>
+        <v>0.3357794316</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1582,11 +1582,11 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.4061359055</v>
+        <v>0.2306579926</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1.0677602318</v>
+        <v>0.5964571469</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -1652,11 +1652,11 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0.0508945148</v>
+        <v>1.5567178893</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1683,15 +1683,15 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>10.0322759408</v>
+        <v>0.0744791948</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1722,11 +1722,11 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>2.9835078</v>
+        <v>14.5273533687</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1757,11 +1757,11 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>2.7783847</v>
+        <v>4.3180501</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1788,15 +1788,15 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>AWS Security Hub</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>23.30692</v>
+        <v>4.0225003</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>AWS Step Functions</t>
+          <t>AWS Security Hub</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0.0001789178</v>
+        <v>32.58619</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1858,11 +1858,11 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>AWS Support (Enterprise)</t>
+          <t>AWS Step Functions</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>13650</v>
+        <v>0.0002569943</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1893,11 +1893,11 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>AWS Systems Manager</t>
+          <t>AWS Support (Enterprise)</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>0.0105105</v>
+        <v>13650</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>AWS Transfer Family</t>
+          <t>AWS Systems Manager</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>15.0591170879</v>
+        <v>0.0150969</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1963,11 +1963,11 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Transfer Family</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>7.8537898356</v>
+        <v>21.6319267379</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2002,11 +2002,11 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>0.821378775</v>
+        <v>11.1950016179</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2037,11 +2037,11 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>51.108165507</v>
+        <v>1.182235005</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2068,15 +2068,15 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>AWS X-Ray</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>2.29894665</v>
+        <v>107.698572933</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2103,11 +2103,11 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Amazon API Gateway</t>
+          <t>AWS X-Ray</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>5.7769830897</v>
+        <v>3.64828555</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2138,11 +2138,11 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Amazon Athena</t>
+          <t>Amazon API Gateway</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0.5223673</v>
+        <v>9.212077580300001</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2173,11 +2173,11 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon Athena</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>710.3274292351</v>
+        <v>0.77862785</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2212,11 +2212,11 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>0.150842429</v>
+        <v>1326.5748744233</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2247,11 +2247,11 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.1559308879</v>
+        <v>0.2197681495</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2282,11 +2282,11 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>269.9963410672</v>
+        <v>0.2629592505</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -2317,11 +2317,11 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>1.141e-07</v>
+        <v>467.7159002028</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2348,15 +2348,15 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Amazon Cognito</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>15.56555</v>
+        <v>0.0013760456</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -2383,15 +2383,15 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Amazon Detective</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>9.237963243799999</v>
+        <v>2.8928e-06</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -2418,11 +2418,11 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Amazon DevOps Guru</t>
+          <t>Amazon Cognito</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>49.1855</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2453,11 +2453,11 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon Detective</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.0105504999</v>
+        <v>13.0126819548</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2488,15 +2488,15 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon DevOps Guru</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>24.6249580359</v>
+        <v>0</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2527,11 +2527,11 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>19.8403232965</v>
+        <v>0.0144760151</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2558,15 +2558,15 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.008630713</v>
+        <v>36.9679208351</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2593,15 +2593,15 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0.9196871958</v>
+        <v>30.9215243553</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2632,11 +2632,11 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>6.897053862</v>
+        <v>1.0310055881</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2663,15 +2663,15 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>11.4883836485</v>
+        <v>0.983823437</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2698,15 +2698,15 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.002462724</v>
+        <v>10.244869415</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2737,11 +2737,11 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.0074896195</v>
+        <v>16.4972156929</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2772,11 +2772,11 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.0270445285</v>
+        <v>0.0035373672</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -2807,11 +2807,11 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>55.473849277</v>
+        <v>0.0107578171</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -2838,15 +2838,15 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>3909.442409557</v>
+        <v>0.0388457773</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2873,15 +2873,15 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>458.5399</v>
+        <v>79.70371869420001</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2912,11 +2912,11 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>361.14624</v>
+        <v>4102.789498314</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2943,15 +2943,15 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1944.7176441798</v>
+        <v>589.3069</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2978,15 +2978,15 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>0.0469677408</v>
+        <v>463.35744</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Environment$PSFalcon</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3017,11 +3017,11 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.0815493545</v>
+        <v>2887.62257578</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3052,11 +3052,11 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>1.1741935488</v>
+        <v>0.0704516112</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Environment$management</t>
+          <t>Environment$PSFalcon</t>
         </is>
       </c>
     </row>
@@ -3087,11 +3087,11 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>99.2576587848</v>
+        <v>0.1355839624</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3122,11 +3122,11 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0.6028407284</v>
+        <v>1.7612903232</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$management</t>
         </is>
       </c>
     </row>
@@ -3157,11 +3157,11 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>423.1940005737</v>
+        <v>145.5675130573</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3192,11 +3192,11 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>6.788442341</v>
+        <v>1.1969264753</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3223,15 +3223,15 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>1782.8750289954</v>
+        <v>636.1890221334</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3258,15 +3258,15 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>4.245696</v>
+        <v>9.763163329999999</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3297,11 +3297,11 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>569.4565021329</v>
+        <v>2585.9437890123</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3332,11 +3332,11 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>6.840288</v>
+        <v>6.132672</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>4596.0203044544</v>
+        <v>821.7027967645</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3402,11 +3402,11 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>4.2260410254</v>
+        <v>9.880416</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3433,15 +3433,15 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>619.4729096024</v>
+        <v>7304.6266379785</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3468,15 +3468,15 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>68.3201314107</v>
+        <v>6.1042813167</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3503,15 +3503,15 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Container Service</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>45.045</v>
+        <v>908.810423105</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3542,11 +3542,11 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>45.045</v>
+        <v>98.1218654481</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3573,15 +3573,15 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Amazon Elastic File System</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>13.7493395872</v>
+        <v>63.7185724175</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3608,15 +3608,15 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>494.994784906</v>
+        <v>64.70099999999999</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3643,15 +3643,15 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic File System</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>1.1261356389</v>
+        <v>19.7493720902</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3682,11 +3682,11 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>1.1317689184</v>
+        <v>756.0586982717</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3717,11 +3717,11 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>20.107772335</v>
+        <v>1.6175413941</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3752,11 +3752,11 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>3.3795696874</v>
+        <v>1.6255226113</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3787,11 +3787,11 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>153.84727815</v>
+        <v>28.886169944</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3822,11 +3822,11 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>1.1309875249</v>
+        <v>4.8542349917</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3853,15 +3853,15 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Amazon Glacier</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>0.1515165654</v>
+        <v>221.8793086823</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3888,15 +3888,15 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Amazon GuardDuty</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>354.8341804816</v>
+        <v>1.6251116478</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3923,11 +3923,11 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Amazon Kinesis</t>
+          <t>Amazon Glacier</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>8.9273561123</v>
+        <v>0.2272748375</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3958,11 +3958,11 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Amazon Lightsail</t>
+          <t>Amazon GuardDuty</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>0.6869659406</v>
+        <v>541.1111519861</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3993,11 +3993,11 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Amazon Location Service</t>
+          <t>Amazon Kinesis</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>8.19e-05</v>
+        <v>12.8913286705</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4028,11 +4028,11 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Lightsail</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>4.4948610899</v>
+        <v>0.9893689412</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4063,15 +4063,15 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Location Service</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>15.8240707639</v>
+        <v>0.000163345</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4102,11 +4102,11 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>15.7564785574</v>
+        <v>6.4562823783</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4133,15 +4133,15 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Amazon Macie</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>0.149604</v>
+        <v>22.732614305</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4168,15 +4168,15 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F107" t="n">
-        <v>8.19</v>
+        <v>22.6377912779</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4203,15 +4203,15 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon Macie</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>8.19</v>
+        <v>0.224406</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Amazon Managed Streaming for Apache Kafka</t>
+          <t>Amazon Managed Grafana</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>5.2372900042</v>
+        <v>8.19</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4273,11 +4273,11 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Amazon Managed Streaming for Apache Kafka</t>
+          <t>Amazon Managed Grafana</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>13.855131609</v>
+        <v>8.19</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4308,11 +4308,11 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Streaming for Apache Kafka</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>616.616</v>
+        <v>7.5226492768</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4343,11 +4343,11 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Streaming for Apache Kafka</t>
         </is>
       </c>
       <c r="F112" t="n">
-        <v>198.198</v>
+        <v>19.9010072202</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4382,11 +4382,11 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>198.198</v>
+        <v>885.6848</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4413,15 +4413,15 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Amazon Neptune</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>0.2778967877</v>
+        <v>284.6844</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4448,15 +4448,15 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>80.2382045778</v>
+        <v>284.6844</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4483,15 +4483,15 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Neptune</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>824.5365767909</v>
+        <v>0.4029878062</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4522,11 +4522,11 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>2208.3531605267</v>
+        <v>115.2512187989</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4557,11 +4557,11 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>8.3984241885</v>
+        <v>1184.3343484908</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4588,15 +4588,15 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Amazon Personalize</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>90.0924705783</v>
+        <v>3171.9982233156</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4623,15 +4623,15 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Amazon QuickSight</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>4.299940579</v>
+        <v>12.0631920334</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -4658,11 +4658,11 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Amazon Redshift</t>
+          <t>Amazon Personalize</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>28.1662449537</v>
+        <v>148.4655642201</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4693,11 +4693,11 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon QuickSight</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>13328.4435884469</v>
+        <v>6.1762782862</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -4728,15 +4728,15 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon Redshift</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>0.0001038016</v>
+        <v>40.4569700241</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4767,11 +4767,11 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>282.129836761</v>
+        <v>15290.9927174139</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4802,11 +4802,11 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>954.6231298117</v>
+        <v>0.0001567616</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -4833,15 +4833,15 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>206.3270536365</v>
+        <v>412.0279804297</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4868,15 +4868,15 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F127" t="n">
-        <v>0.10104458</v>
+        <v>1389.370760303</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4907,11 +4907,11 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>0.091</v>
+        <v>269.0163376948</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4942,11 +4942,11 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>0.091</v>
+        <v>0.105752192</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -4977,11 +4977,11 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>0.455</v>
+        <v>0.091</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5012,11 +5012,11 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>0.09102366000000001</v>
+        <v>0.091</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5047,11 +5047,11 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>4.440533552</v>
+        <v>0.455</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -5082,11 +5082,11 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>2.40111326</v>
+        <v>0.09102912000000001</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5117,11 +5117,11 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>0.091017836</v>
+        <v>4.674641972</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Environment$sandbox</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5152,11 +5152,11 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>0.091004368</v>
+        <v>2.90434144</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5187,11 +5187,11 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>0.091</v>
+        <v>0.091018928</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Environment$test</t>
+          <t>Environment$sandbox</t>
         </is>
       </c>
     </row>
@@ -5218,15 +5218,15 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Amazon SageMaker</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F137" t="n">
-        <v>307.2953349085</v>
+        <v>0.091005824</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -5253,15 +5253,15 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Amazon Simple Email Service</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F138" t="n">
-        <v>0.8287508401</v>
+        <v>0.091</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$test</t>
         </is>
       </c>
     </row>
@@ -5288,11 +5288,11 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon SageMaker</t>
         </is>
       </c>
       <c r="F139" t="n">
-        <v>0.8644049343</v>
+        <v>439.7274073308</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -5323,15 +5323,15 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Simple Email Service</t>
         </is>
       </c>
       <c r="F140" t="n">
-        <v>1.4657e-05</v>
+        <v>1.2830111239</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5362,11 +5362,11 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>2.73e-06</v>
+        <v>1.4628569636</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5397,11 +5397,11 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>4.368e-05</v>
+        <v>0.0002417227</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5463,15 +5463,15 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F144" t="n">
-        <v>1.9622152808</v>
+        <v>7.735e-05</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5498,15 +5498,15 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F145" t="n">
-        <v>5.096e-06</v>
+        <v>4.55e-06</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5537,11 +5537,11 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>0.064992966</v>
+        <v>3.0977483158</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5572,11 +5572,11 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>0.09382219560000001</v>
+        <v>8.372e-06</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5603,15 +5603,15 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>2373.2298518776</v>
+        <v>0.09886583340000001</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5638,15 +5638,15 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F149" t="n">
-        <v>0.0047291087</v>
+        <v>0.1402567174</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5677,11 +5677,11 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>6.07763e-05</v>
+        <v>3611.7195531926</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5712,11 +5712,11 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0.0051737695</v>
+        <v>0.0066036155</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Environment$POC</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5747,11 +5747,11 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>0.0024570832</v>
+        <v>8.054670000000001e-05</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5782,11 +5782,11 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>6.74258e-05</v>
+        <v>0.0076658577</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$POC</t>
         </is>
       </c>
     </row>
@@ -5817,11 +5817,11 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.0001859363</v>
+        <v>0.00355445</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5852,11 +5852,11 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>1.4072559182</v>
+        <v>8.85677e-05</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5887,11 +5887,11 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>0.0046270377</v>
+        <v>0.0002619708</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5922,11 +5922,11 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>107.0157431683</v>
+        <v>2.0952127066</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5957,11 +5957,11 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.2374201709</v>
+        <v>0.007927093099999999</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5992,11 +5992,11 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>1137.405769717</v>
+        <v>158.4764249752</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6027,11 +6027,11 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>6.26678e-05</v>
+        <v>0.3416719579</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6062,11 +6062,11 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0.0002272991</v>
+        <v>1708.1260488262</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6093,15 +6093,15 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Amazon Simple Workflow Service</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>8.710000000000001e-08</v>
+        <v>8.27122e-05</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -6128,15 +6128,15 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Amazon SimpleDB</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>1.0349e-06</v>
+        <v>0.000320848</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -6163,11 +6163,11 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon Simple Workflow Service</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>698.550931067</v>
+        <v>1.223e-07</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -6198,15 +6198,15 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon SimpleDB</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>7.4165</v>
+        <v>1.4489e-06</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6237,11 +6237,11 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>0.2366</v>
+        <v>1033.4077562641</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6272,11 +6272,11 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>10.3740079244</v>
+        <v>10.738</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6307,11 +6307,11 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>6.8461300136</v>
+        <v>0.3458</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6338,15 +6338,15 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Amazon WorkSpaces</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F169" t="n">
-        <v>216.2887999382</v>
+        <v>15.0059114662</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6373,15 +6373,15 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>728.0173403868</v>
+        <v>9.827890264500001</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -6408,15 +6408,15 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon WorkSpaces</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>66.17393232800001</v>
+        <v>216.2887999382</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6447,11 +6447,11 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>210.5643900976</v>
+        <v>1089.0819689727</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6478,15 +6478,15 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>AmazonWorkMail</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>13.185215043</v>
+        <v>94.3789460568</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6513,15 +6513,15 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>0.1513264296</v>
+        <v>363.643716153</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6548,11 +6548,11 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>AmazonWorkMail</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>27081.6</v>
+        <v>18.9387634254</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6583,13 +6583,83 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
+          <t>CloudWatch Events</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>0.1938018833</v>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F177" t="n">
+        <v>27081.6</v>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
           <t>Tax</t>
         </is>
       </c>
-      <c r="F176" t="n">
-        <v>702.15</v>
-      </c>
-      <c r="G176" t="inlineStr">
+      <c r="F178" t="n">
+        <v>993.16</v>
+      </c>
+      <c r="G178" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>

<commit_message>
Finish the ML Time Series but no Suppot for Terraform on Work Laptop
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_MAR_2025.xlsx
+++ b/Monthly_Cost_For_MAR_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0007356137</v>
+        <v>0.0020117602</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.1648431505</v>
+        <v>0.5059119345</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>17.1435510421</v>
+        <v>45.7319203341</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.0546</v>
+        <v>0.1456</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -668,11 +668,11 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AWS CloudTrail</t>
+          <t>AWS CloudFormation</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>341.3149955157</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -703,11 +703,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>AWS Config</t>
+          <t>AWS CloudTrail</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>221.67964</v>
+        <v>1007.5056432142</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -738,11 +738,11 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>AWS Cost Explorer</t>
+          <t>AWS CodeCommit</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2.4479</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -773,11 +773,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>AWS DataSync</t>
+          <t>AWS CodePipeline</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1.2590381087</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -808,11 +808,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>AWS Database Migration Service</t>
+          <t>AWS Config</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>267.380329249</v>
+        <v>626.7898</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -843,15 +843,15 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AWS Database Migration Service</t>
+          <t>AWS Cost Explorer</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>32.7427256622</v>
+        <v>3.9858</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -878,11 +878,11 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>AWS Directory Service</t>
+          <t>AWS DataSync</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>52.4658973758</v>
+        <v>3.4905133161</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -913,11 +913,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>AWS Elemental MediaLive</t>
+          <t>AWS Database Migration Service</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2.8756</v>
+        <v>765.0738501098</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -948,15 +948,15 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AWS Elemental MediaStore</t>
+          <t>AWS Database Migration Service</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1.78448e-05</v>
+        <v>89.109949587</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -983,11 +983,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AWS End User Messaging</t>
+          <t>AWS Directory Service</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.2898790292</v>
+        <v>142.1404807761</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1018,11 +1018,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AWS Global Accelerator</t>
+          <t>AWS Elemental MediaLive</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>7.826</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1053,15 +1053,15 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AWS Global Accelerator</t>
+          <t>AWS Elemental MediaStore</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3.5948707742</v>
+        <v>4.97776e-05</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1088,11 +1088,11 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AWS Glue</t>
+          <t>AWS End User Messaging</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.2381931552</v>
+        <v>0.788911282</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1123,11 +1123,11 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AWS Key Management Service</t>
+          <t>AWS Global Accelerator</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>19.5298095382</v>
+        <v>0</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1158,15 +1158,15 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>AWS Key Management Service</t>
+          <t>AWS Global Accelerator</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.1920675582</v>
+        <v>9.783088405499999</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1193,15 +1193,15 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>AWS Key Management Service</t>
+          <t>AWS Glue</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.0955015074</v>
+        <v>0.5034361332</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1232,11 +1232,11 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.0967846857</v>
+        <v>52.2519995057</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1267,11 +1267,11 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>7.9670947749</v>
+        <v>0.5290444092</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1302,11 +1302,11 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>6.2882044014</v>
+        <v>0.2607971979</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1337,11 +1337,11 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.0954032274</v>
+        <v>0.2634236145</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Environment$sandbox</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -1372,11 +1372,11 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.1908064548</v>
+        <v>21.1457911857</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1407,11 +1407,11 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.1911149448</v>
+        <v>17.1873993</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1438,15 +1438,15 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>AWS Lambda</t>
+          <t>AWS Key Management Service</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>171.1901145307</v>
+        <v>0.2605269279</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$sandbox</t>
         </is>
       </c>
     </row>
@@ -1473,15 +1473,15 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>AWS Lambda</t>
+          <t>AWS Key Management Service</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>2.00276e-05</v>
+        <v>0.5222715140999999</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Environment$Development</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -1508,15 +1508,15 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>AWS Lambda</t>
+          <t>AWS Key Management Service</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1.9678661285</v>
+        <v>0.3715139349</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1547,11 +1547,11 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.3357794316</v>
+        <v>538.4713838818</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1582,11 +1582,11 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.2306579926</v>
+        <v>3.77878e-05</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Development</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0.5964571469</v>
+        <v>5.73858336</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1652,11 +1652,11 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1.5567178893</v>
+        <v>0.5108436193</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1687,11 +1687,11 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0.0744791948</v>
+        <v>0.6470954957</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1718,15 +1718,15 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>14.5273533687</v>
+        <v>1.6902541084</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -1753,15 +1753,15 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>4.3180501</v>
+        <v>4.3648785228</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1788,15 +1788,15 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>4.0225003</v>
+        <v>0.207891652</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>AWS Security Hub</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>32.58619</v>
+        <v>39.0309104912</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1858,15 +1858,15 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>AWS Step Functions</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.0002569943</v>
+        <v>11.7931177</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1893,15 +1893,15 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>AWS Support (Enterprise)</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>13650</v>
+        <v>11.1550894</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>AWS Systems Manager</t>
+          <t>AWS Security Hub</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0.0150969</v>
+        <v>84.64091999999999</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1963,11 +1963,11 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AWS Transfer Family</t>
+          <t>AWS Service Catalog</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>21.6319267379</v>
+        <v>0</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1998,11 +1998,11 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Step Functions</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>11.1950016179</v>
+        <v>0.0007299986</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2033,15 +2033,15 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Support (Enterprise)</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>1.182235005</v>
+        <v>19012.3388</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2068,15 +2068,15 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Systems Manager</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>107.698572933</v>
+        <v>0.0410865</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2103,11 +2103,11 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>AWS X-Ray</t>
+          <t>AWS Transfer Family</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>3.64828555</v>
+        <v>58.8458784531</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2138,11 +2138,11 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Amazon API Gateway</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>9.212077580300001</v>
+        <v>29.9996460778</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2173,15 +2173,15 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Amazon Athena</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>0.77862785</v>
+        <v>3.222744273</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2208,15 +2208,15 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>1326.5748744233</v>
+        <v>393.566077107</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2243,15 +2243,15 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>AWS X-Ray</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.2197681495</v>
+        <v>11.89788873</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2278,15 +2278,15 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon API Gateway</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>0.2629592505</v>
+        <v>27.6643891611</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2313,15 +2313,15 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon Athena</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>467.7159002028</v>
+        <v>2.32676535</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2352,11 +2352,11 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>0.0013760456</v>
+        <v>4373.35464493</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2387,11 +2387,11 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>2.8928e-06</v>
+        <v>0.597750253</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2418,15 +2418,15 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Amazon Cognito</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>49.1855</v>
+        <v>0.7737739338</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -2453,15 +2453,15 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Amazon Detective</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>13.0126819548</v>
+        <v>1551.2623494517</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2488,15 +2488,15 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Amazon DevOps Guru</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>0.0062217681</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -2523,15 +2523,15 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.0144760151</v>
+        <v>0.0003291154</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -2558,15 +2558,15 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon Cognito</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>36.9679208351</v>
+        <v>70.42489999999999</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2593,15 +2593,15 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon Detective</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>30.9215243553</v>
+        <v>35.0186032576</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2628,11 +2628,11 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DevOps Guru</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>1.0310055881</v>
+        <v>0</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2663,15 +2663,15 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0.983823437</v>
+        <v>0.0408870114</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2698,15 +2698,15 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>10.244869415</v>
+        <v>101.680957946</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2733,15 +2733,15 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>16.4972156929</v>
+        <v>90.3512204581</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2768,15 +2768,15 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.0035373672</v>
+        <v>25.7712465812</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2803,15 +2803,15 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0.0107578171</v>
+        <v>2.8364754002</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2838,15 +2838,15 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>0.0388457773</v>
+        <v>32.3750329533</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2877,11 +2877,11 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>79.70371869420001</v>
+        <v>44.5184758776</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2908,15 +2908,15 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>4102.789498314</v>
+        <v>0.009627012000000001</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -2943,15 +2943,15 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>589.3069</v>
+        <v>0.0224688585</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -2978,15 +2978,15 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>463.35744</v>
+        <v>0.1057191293</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3013,15 +3013,15 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>2887.62257578</v>
+        <v>217.2360829049</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3048,15 +3048,15 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.0704516112</v>
+        <v>5991.4524700411</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Environment$PSFalcon</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3083,15 +3083,15 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.1355839624</v>
+        <v>1836.0251</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3118,15 +3118,15 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>1.7612903232</v>
+        <v>1465.0272</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Environment$management</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3157,11 +3157,11 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>145.5675130573</v>
+        <v>7534.8793976299</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3192,11 +3192,11 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1.1969264753</v>
+        <v>0.2035268768</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$PSFalcon</t>
         </is>
       </c>
     </row>
@@ -3227,11 +3227,11 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>636.1890221334</v>
+        <v>0.4450753682</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3262,11 +3262,11 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>9.763163329999999</v>
+        <v>5.0881720448</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$management</t>
         </is>
       </c>
     </row>
@@ -3293,15 +3293,15 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>2585.9437890123</v>
+        <v>389.5258609149</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3328,15 +3328,15 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>6.132672</v>
+        <v>4.7593394032</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3363,15 +3363,15 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>821.7027967645</v>
+        <v>1818.7366256384</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3398,15 +3398,15 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>9.880416</v>
+        <v>11.3939560323</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3437,11 +3437,11 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>7304.6266379785</v>
+        <v>7008.6479934922</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3472,11 +3472,11 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>6.1042813167</v>
+        <v>16.825536</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3503,15 +3503,15 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>908.810423105</v>
+        <v>2172.6564059364</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3538,15 +3538,15 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>98.1218654481</v>
+        <v>27.107808</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3573,15 +3573,15 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>63.7185724175</v>
+        <v>21761.1822462207</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3608,15 +3608,15 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>64.70099999999999</v>
+        <v>16.7476413621</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3643,11 +3643,11 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Amazon Elastic File System</t>
+          <t>Amazon Elastic Container Service</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>19.7493720902</v>
+        <v>2512.6026769245</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3678,11 +3678,11 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>756.0586982717</v>
+        <v>267.0669492571</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3713,15 +3713,15 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>1.6175413941</v>
+        <v>162.7265724175</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3748,15 +3748,15 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>1.6255226113</v>
+        <v>176.085</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3783,15 +3783,15 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic File System</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>28.886169944</v>
+        <v>53.750589351</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3822,11 +3822,11 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>4.8542349917</v>
+        <v>2082.7317767359</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3857,11 +3857,11 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>221.8793086823</v>
+        <v>4.4021790527</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3892,11 +3892,11 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>1.6251116478</v>
+        <v>4.4220253359</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3923,15 +3923,15 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Amazon Glacier</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>0.2272748375</v>
+        <v>78.4013630396</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3958,15 +3958,15 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Amazon GuardDuty</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>541.1111519861</v>
+        <v>13.2108120111</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3993,15 +3993,15 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Amazon Kinesis</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>12.8913286705</v>
+        <v>608.1837127738</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4028,15 +4028,15 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Amazon Lightsail</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>0.9893689412</v>
+        <v>4.4268112593</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -4063,11 +4063,11 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Amazon Location Service</t>
+          <t>Amazon Glacier</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0.000163345</v>
+        <v>0.6818257149</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4098,11 +4098,11 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon GuardDuty</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>6.4562823783</v>
+        <v>1328.4330538686</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4133,15 +4133,15 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Inspector</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>22.732614305</v>
+        <v>0.546</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4168,15 +4168,15 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Kinesis</t>
         </is>
       </c>
       <c r="F107" t="n">
-        <v>22.6377912779</v>
+        <v>35.2769341851</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4203,11 +4203,11 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Amazon Macie</t>
+          <t>Amazon Lightsail</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>0.224406</v>
+        <v>2.6983114987</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon Location Service</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>8.19</v>
+        <v>0.000426335</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4273,15 +4273,15 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>8.19</v>
+        <v>17.571800324</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4308,15 +4308,15 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Amazon Managed Streaming for Apache Kafka</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>7.5226492768</v>
+        <v>62.5943663453</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4343,15 +4343,15 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Amazon Managed Streaming for Apache Kafka</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F112" t="n">
-        <v>19.9010072202</v>
+        <v>62.343399767</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4378,11 +4378,11 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Macie</t>
         </is>
       </c>
       <c r="F113" t="n">
-        <v>885.6848</v>
+        <v>0.5984159999999999</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4413,15 +4413,15 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Grafana</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>284.6844</v>
+        <v>8.19</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4448,15 +4448,15 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Streaming for Apache Kafka</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>284.6844</v>
+        <v>20.4730602709</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4483,15 +4483,15 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Amazon Neptune</t>
+          <t>Amazon Managed Streaming for Apache Kafka</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>0.4029878062</v>
+        <v>30.0085511897</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4518,11 +4518,11 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F117" t="n">
-        <v>115.2512187989</v>
+        <v>2410.4629264275</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -4553,11 +4553,11 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F118" t="n">
-        <v>1184.3343484908</v>
+        <v>773.2600150275</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -4588,11 +4588,11 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>3171.9982233156</v>
+        <v>773.555181399</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4623,15 +4623,15 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Neptune</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>12.0631920334</v>
+        <v>1.233556477</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4658,11 +4658,11 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Amazon Personalize</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>148.4655642201</v>
+        <v>305.3599665757</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4693,15 +4693,15 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Amazon QuickSight</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>6.1762782862</v>
+        <v>3095.0426899229</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4728,15 +4728,15 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Amazon Redshift</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>40.4569700241</v>
+        <v>8632.6538731824</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4763,15 +4763,15 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F124" t="n">
-        <v>15290.9927174139</v>
+        <v>13.8955785969</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -4798,15 +4798,15 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon Personalize</t>
         </is>
       </c>
       <c r="F125" t="n">
-        <v>0.0001567616</v>
+        <v>450.3447129617</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4833,15 +4833,15 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon QuickSight</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>412.0279804297</v>
+        <v>16.740561666</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4868,15 +4868,15 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon Redshift</t>
         </is>
       </c>
       <c r="F127" t="n">
-        <v>1389.370760303</v>
+        <v>110.047410599</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4903,11 +4903,11 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F128" t="n">
-        <v>269.0163376948</v>
+        <v>26073.4746766282</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4938,15 +4938,15 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F129" t="n">
-        <v>0.105752192</v>
+        <v>0.0004491008</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -4973,15 +4973,15 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>0.091</v>
+        <v>1069.2493367896</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5008,15 +5008,15 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F131" t="n">
-        <v>0.091</v>
+        <v>4499.217748528</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5047,11 +5047,11 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>0.455</v>
+        <v>608.2207107523</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5082,11 +5082,11 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>0.09102912000000001</v>
+        <v>0.132160028</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5117,11 +5117,11 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>4.674641972</v>
+        <v>0.091</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5152,11 +5152,11 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>2.90434144</v>
+        <v>0.091</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5187,11 +5187,11 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>0.091018928</v>
+        <v>0.455</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Environment$sandbox</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -5222,11 +5222,11 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>0.091005824</v>
+        <v>0.091066248</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5257,11 +5257,11 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>0.091</v>
+        <v>6.08215608</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Environment$test</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5288,15 +5288,15 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Amazon SageMaker</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F139" t="n">
-        <v>439.7274073308</v>
+        <v>5.616782808</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5323,15 +5323,15 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Amazon Simple Email Service</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F140" t="n">
-        <v>1.2830111239</v>
+        <v>0.09104076799999999</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$sandbox</t>
         </is>
       </c>
     </row>
@@ -5358,15 +5358,15 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F141" t="n">
-        <v>1.4628569636</v>
+        <v>0.091011284</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -5393,15 +5393,15 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F142" t="n">
-        <v>0.0002417227</v>
+        <v>0.091</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$test</t>
         </is>
       </c>
     </row>
@@ -5428,15 +5428,15 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon SageMaker</t>
         </is>
       </c>
       <c r="F143" t="n">
-        <v>3.64e-06</v>
+        <v>1094.0872851627</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5463,15 +5463,15 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Simple Email Service</t>
         </is>
       </c>
       <c r="F144" t="n">
-        <v>7.735e-05</v>
+        <v>3.6053860077</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5502,11 +5502,11 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>4.55e-06</v>
+        <v>4.8268257453</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5533,15 +5533,15 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F146" t="n">
-        <v>3.0977483158</v>
+        <v>0.00247834</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5568,15 +5568,15 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F147" t="n">
-        <v>8.372e-06</v>
+        <v>1.5015e-05</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5603,15 +5603,15 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>0.09886583340000001</v>
+        <v>0.00027482</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5638,11 +5638,11 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F149" t="n">
-        <v>0.1402567174</v>
+        <v>1.5925e-05</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -5673,11 +5673,11 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F150" t="n">
-        <v>3611.7195531926</v>
+        <v>9.4133433677</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -5708,15 +5708,15 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0.0066036155</v>
+        <v>2.6572e-05</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5743,15 +5743,15 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F152" t="n">
-        <v>8.054670000000001e-05</v>
+        <v>0.2907592634</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5778,15 +5778,15 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F153" t="n">
-        <v>0.0076658577</v>
+        <v>0.403406838</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Environment$POC</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5817,11 +5817,11 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.00355445</v>
+        <v>10701.6687828151</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5852,11 +5852,11 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>8.85677e-05</v>
+        <v>0.0212861422</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5887,11 +5887,11 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>0.0002619708</v>
+        <v>0.0002434963</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5922,11 +5922,11 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>2.0952127066</v>
+        <v>0.0226325022</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$POC</t>
         </is>
       </c>
     </row>
@@ -5957,11 +5957,11 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.007927093099999999</v>
+        <v>0.0100954166</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5992,11 +5992,11 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>158.4764249752</v>
+        <v>0.0002401577</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -6027,11 +6027,11 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0.3416719579</v>
+        <v>0.0007210909</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -6062,11 +6062,11 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>1708.1260488262</v>
+        <v>6.2229599845</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -6097,11 +6097,11 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>8.27122e-05</v>
+        <v>0.0249400494</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -6132,11 +6132,11 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>0.000320848</v>
+        <v>462.7666659891</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6163,15 +6163,15 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Amazon Simple Workflow Service</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>1.223e-07</v>
+        <v>1.1869538328</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6198,15 +6198,15 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Amazon SimpleDB</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>1.4489e-06</v>
+        <v>5108.171065668</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6233,15 +6233,15 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>1033.4077562641</v>
+        <v>0.0002525345</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -6268,15 +6268,15 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>10.738</v>
+        <v>0.0023887284</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -6303,15 +6303,15 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon Simple Workflow Service</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>0.3458</v>
+        <v>3.168e-07</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6338,15 +6338,15 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon SimpleDB</t>
         </is>
       </c>
       <c r="F169" t="n">
-        <v>15.0059114662</v>
+        <v>3.726e-06</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6377,11 +6377,11 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>9.827890264500001</v>
+        <v>2834.6715585556</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6408,15 +6408,15 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Amazon WorkSpaces</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>216.2887999382</v>
+        <v>36.0502288689</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6443,15 +6443,15 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>1089.0819689727</v>
+        <v>0.9646</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6478,15 +6478,15 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>94.3789460568</v>
+        <v>41.0261842759</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6513,15 +6513,15 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>363.643716153</v>
+        <v>26.7409579993</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -6548,15 +6548,15 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>AmazonWorkMail</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>18.9387634254</v>
+        <v>0.0360549645</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -6583,11 +6583,11 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>Amazon WorkSpaces</t>
         </is>
       </c>
       <c r="F176" t="n">
-        <v>0.1938018833</v>
+        <v>216.2887999382</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -6618,11 +6618,11 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F177" t="n">
-        <v>27081.6</v>
+        <v>3098.0197477051</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -6653,13 +6653,223 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
+          <t>AmazonCloudWatch</t>
+        </is>
+      </c>
+      <c r="F178" t="n">
+        <v>247.6090766456</v>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Environment$nonprod</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>AmazonCloudWatch</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>1171.5424017521</v>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>Environment$prod</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>AmazonWorkMail</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>51.542204259</v>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>CloudWatch Events</t>
+        </is>
+      </c>
+      <c r="F181" t="n">
+        <v>0.3817603001</v>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>CodeBuild</t>
+        </is>
+      </c>
+      <c r="F182" t="n">
+        <v>0</v>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F183" t="n">
+        <v>27081.6</v>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
           <t>Tax</t>
         </is>
       </c>
-      <c r="F178" t="n">
-        <v>993.16</v>
-      </c>
-      <c r="G178" t="inlineStr">
+      <c r="F184" t="n">
+        <v>2736.71</v>
+      </c>
+      <c r="G184" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>

<commit_message>
Forcasting  wiht March 2025 Completed
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_MAR_2025.xlsx
+++ b/Monthly_Cost_For_MAR_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G188"/>
+  <dimension ref="A1:G189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0026928806</v>
+        <v>0.0028018086</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.6056494567</v>
+        <v>2.0463308678</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>145.1362091929</v>
+        <v>180.3368047471</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.455</v>
+        <v>0.5642</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2846.8346321871</v>
+        <v>3477.8805483997</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1779.64332</v>
+        <v>2160.479776</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>9.1637</v>
+        <v>10.7653</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>9.911063437599999</v>
+        <v>12.1928130541</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2192.2832115722</v>
+        <v>2742.4274689906</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>250.751253489</v>
+        <v>308.3618720592</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>401.2783488056</v>
+        <v>494.2488148973</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>22.022</v>
+        <v>27.0816</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.0001413496</v>
+        <v>0.0001746912</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>2.219959654</v>
+        <v>2.7299999712</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>27.5280884055</v>
+        <v>33.8525884055</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1.4218856652</v>
+        <v>1.6878849988</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>137.6810856633</v>
+        <v>168.0155514646</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1.4998278066</v>
+        <v>1.8502753389</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.7370816166</v>
+        <v>0.9072888903</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.7388179749</v>
+        <v>0.9103602969</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>56.64256743</v>
+        <v>68.9214985965</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>48.3850819263</v>
+        <v>59.5915105293</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1.4750970498</v>
+        <v>1.8163470555</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.8479157436</v>
+        <v>1.0181230173</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1581.1451538225</v>
+        <v>1939.3155227632</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>2.4401763515</v>
+        <v>4.4612902179</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>12.2663420905</v>
+        <v>12.7403776257</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.9596212247</v>
+        <v>1.119267595</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1.7614544851</v>
+        <v>2.1659813328</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>4.7324040997</v>
+        <v>5.8329866203</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>12.415185232</v>
+        <v>15.3065778595</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.5916141718</v>
+        <v>0.7272765634</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>107.1384779076</v>
+        <v>131.3261771349</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>35.40219865</v>
+        <v>44.1277837</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>31.80027305</v>
+        <v>39.15264535</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>205.2861447</v>
+        <v>246.0860857</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>0.0019987752</v>
+        <v>0.0024509599</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>38142.5317</v>
+        <v>47910.0531</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0.1156155</v>
+        <v>0.1421784</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>165.5452699181</v>
+        <v>203.5935941269</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>84.1476935461</v>
+        <v>103.7293923497</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>9.050641257000001</v>
+        <v>11.251596846</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>1189.558646115</v>
+        <v>1462.442571534</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>36.849056335</v>
+        <v>45.729166665</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>141.7014989332</v>
+        <v>194.4478352723</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>7.14511525</v>
+        <v>9.22269075</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>12992.7335956316</v>
+        <v>16083.1858318378</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1.5736725478</v>
+        <v>1.979390182</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>1.8460789879</v>
+        <v>2.2836541628</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>4629.5686404032</v>
+        <v>5650.0261872015</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.0405661541</v>
+        <v>0.0513142004</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2597,7 +2597,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0.0003297183</v>
+        <v>0.0003299388</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>88.16535</v>
+        <v>91.6643</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>99.7707029857</v>
+        <v>122.4148992111</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.116756019</v>
+        <v>0.1456326432</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>281.7727055978</v>
+        <v>331.0394190894</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>260.5844949758</v>
+        <v>316.1518833035</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>70.92140485429999</v>
+        <v>88.9053035525</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>29.3572634896</v>
+        <v>32.4109722525</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>92.73882254190001</v>
+        <v>115.1910049245</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>108.9481932335</v>
+        <v>131.300434798</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>0.027089964</v>
+        <v>0.0333139392</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.2974856015</v>
+        <v>0.3658387128</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>616.7496817071</v>
+        <v>762.410019429</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3122,7 +3122,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>10469.543505993</v>
+        <v>11829.9808148102</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>5181.6008927225</v>
+        <v>6366.1915727225</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>4102.07616</v>
+        <v>5069.67552</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>20924.2129298878</v>
+        <v>25550.8999375845</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>0.5851397708</v>
+        <v>0.7279999824</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>1.2998659926</v>
+        <v>1.6449709013</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>14.6284946288</v>
+        <v>18.2000000064</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>963.4418149035</v>
+        <v>1178.8654541604</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>14.2663311229</v>
+        <v>18.4176347367</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>5168.0732166647</v>
+        <v>6609.9791594171</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>11.8121421994</v>
+        <v>11.9858189794</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>18063.3730105702</v>
+        <v>22057.4479534896</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>47.488896</v>
+        <v>58.496256</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3577,7 +3577,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>6167.9781852418</v>
+        <v>7596.2128298798</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>76.4557005474</v>
+        <v>94.18978054740001</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>61043.7025376628</v>
+        <v>74348.7344910721</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>47.3498228209</v>
+        <v>58.3228530709</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>7093.3431236669</v>
+        <v>8929.612992213701</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>575.4205476175</v>
+        <v>672.1391978189999</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>446.6465724175</v>
+        <v>547.8385724175</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>495.495</v>
+        <v>609.336</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>104.5927697993</v>
+        <v>117.9875281584</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>5818.5502042535</v>
+        <v>7274.0884205006</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>12.3875404599</v>
+        <v>15.2336036063</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>12.4477980653</v>
+        <v>15.306543183</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3997,7 +3997,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>228.8394001091</v>
+        <v>283.9817653767</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>37.1772109613</v>
+        <v>45.7206892604</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>1702.6172055201</v>
+        <v>2085.4655278181</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>12.4828551868</v>
+        <v>15.353543115</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4137,7 +4137,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>1.8939605585</v>
+        <v>2.3485113941</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>2980.6150465655</v>
+        <v>3541.5271874285</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -4207,7 +4207,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>1.638</v>
+        <v>2.184</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>92.0350815697</v>
+        <v>111.0085815697</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4277,7 +4277,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>7.5972946873</v>
+        <v>9.3530927487</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>0.00117845</v>
+        <v>0.00145964</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>49.4404506037</v>
+        <v>60.7987371136</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>174.9758251545</v>
+        <v>214.7853527004</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>174.9749618223</v>
+        <v>217.1947026256</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>1.87005</v>
+        <v>2.318862</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>6782.6916198123</v>
+        <v>8340.7794350924</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>2177.836893242</v>
+        <v>2677.3975613565</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>2178.959181399</v>
+        <v>2679.859581399</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4697,7 +4697,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>3.5491590898</v>
+        <v>4.3989038803</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>810.860409659</v>
+        <v>991.0247776508</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>8403.555475446899</v>
+        <v>10300.27857078</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>24027.019176097</v>
+        <v>29501.7095942519</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>1039.4434390238</v>
+        <v>1216.5276681638</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>47.299346369</v>
+        <v>58.1664689232</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>309.6407540035</v>
+        <v>380.7645021824</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>55434.070934275</v>
+        <v>65407.7473706416</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -5047,7 +5047,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>0.0012773952</v>
+        <v>0.0015760896</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>2951.3210342351</v>
+        <v>3662.3788910858</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -5117,7 +5117,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>14105.810511305</v>
+        <v>17519.3820113986</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -5152,7 +5152,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>1350.7704574094</v>
+        <v>1609.0276297159</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>0.173238884</v>
+        <v>0.185940118</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -5327,7 +5327,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>0.09113995799999999</v>
+        <v>0.091211666</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>8.301310836000001</v>
+        <v>8.982055264</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>10.051382068</v>
+        <v>11.455880254</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>0.09109919</v>
+        <v>0.09116289</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5467,7 +5467,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>0.091020566</v>
+        <v>0.09102384199999999</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -5537,7 +5537,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>2601.4376574929</v>
+        <v>3064.6753392502</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>9.960492848299999</v>
+        <v>12.5530500353</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>14.1537681874</v>
+        <v>17.3476183788</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>0.0061649131</v>
+        <v>0.0073611884</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -5677,7 +5677,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>4.5045e-05</v>
+        <v>5.7785e-05</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -5712,7 +5712,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0.000578305</v>
+        <v>0.00057967</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -5747,7 +5747,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>4.459e-05</v>
+        <v>5.5965e-05</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>27.0380699586</v>
+        <v>33.380357141</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>7.971599999999999e-05</v>
+        <v>9.7916e-05</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -5852,7 +5852,7 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>0.8963782732</v>
+        <v>1.1108250005</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -5887,7 +5887,7 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>1.1858012904</v>
+        <v>1.4582308599</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -5922,7 +5922,7 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>29479.4255286418</v>
+        <v>35713.9919833592</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -5957,7 +5957,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.0611398095</v>
+        <v>0.0758034791</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>0.0005506238</v>
+        <v>0.000595601</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0.0611895273</v>
+        <v>0.0755731889</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -6062,7 +6062,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0.0268916702</v>
+        <v>0.032918627</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>0.0007095253</v>
+        <v>0.0008829575</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>0.0020460985</v>
+        <v>0.0025229292</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -6167,7 +6167,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>16.7615656728</v>
+        <v>20.7017810677</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -6202,7 +6202,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0.0708827266</v>
+        <v>0.0879643681</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>1256.6521693421</v>
+        <v>1548.1385189056</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -6272,7 +6272,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>3.5443671405</v>
+        <v>4.2786203497</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>13849.4790641395</v>
+        <v>17190.5005129313</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0.000707676</v>
+        <v>0.000880776</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -6377,7 +6377,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>0.0041419775</v>
+        <v>0.0047236984</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -6412,7 +6412,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>8.8e-07</v>
+        <v>1.0727e-06</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -6447,7 +6447,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>1.035e-05</v>
+        <v>1.2627e-05</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -6482,7 +6482,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>7743.5562458122</v>
+        <v>9480.8869363131</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -6517,7 +6517,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>115.3952661084</v>
+        <v>144.0966661084</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -6552,7 +6552,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>2.7391</v>
+        <v>3.3852</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>115.3277590552</v>
+        <v>142.0271791409</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>74.9916718427</v>
+        <v>92.174981488</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -6727,7 +6727,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>8870.750314692699</v>
+        <v>10935.7548593658</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>683.432331457</v>
+        <v>835.4517321132</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -6797,7 +6797,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>3706.6949059486</v>
+        <v>4605.8524582718</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>145.037365473</v>
+        <v>178.3599998544</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -6863,11 +6863,11 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>Apache Kafka® &amp; Apache Flink® on Confluent Cloud™ - Annual Commits</t>
         </is>
       </c>
       <c r="F184" t="n">
-        <v>1.5421729825</v>
+        <v>281494.33</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -6898,11 +6898,11 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>CodeBuild</t>
+          <t>CloudWatch Events</t>
         </is>
       </c>
       <c r="F185" t="n">
-        <v>0</v>
+        <v>2.1111231139</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -6933,11 +6933,11 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>NetSPI</t>
+          <t>CodeBuild</t>
         </is>
       </c>
       <c r="F186" t="n">
-        <v>39495</v>
+        <v>0</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -6968,11 +6968,11 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>NetSPI</t>
         </is>
       </c>
       <c r="F187" t="n">
-        <v>27081.6</v>
+        <v>39495</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -7003,13 +7003,48 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F188" t="n">
+        <v>122740.8</v>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
           <t>Tax</t>
         </is>
       </c>
-      <c r="F188" t="n">
-        <v>9956.15</v>
-      </c>
-      <c r="G188" t="inlineStr">
+      <c r="F189" t="n">
+        <v>28693.72</v>
+      </c>
+      <c r="G189" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>